<commit_message>
(Tests) Adding tests to validate files with comments work ok
</commit_message>
<xml_diff>
--- a/tests/Comments.xlsx
+++ b/tests/Comments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\lib\python\sxl\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{E14D036D-85F7-41C6-9AE6-BA3CC7852C69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{83D14788-34A7-40CB-9451-65F9738809A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11925" activeTab="1" xr2:uid="{DB19CD56-1E17-48A7-A928-6B8FE99EB043}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11925" xr2:uid="{DB19CD56-1E17-48A7-A928-6B8FE99EB043}"/>
   </bookViews>
   <sheets>
     <sheet name="no Data" sheetId="1" r:id="rId1"/>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C713BAE6-301E-4837-8B1C-C863A3605AC7}">
   <dimension ref="D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69661599-6179-4729-9DD3-77B0A23D8C88}">
   <dimension ref="B5:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>